<commit_message>
add feature: export to file, minor bugs fix
</commit_message>
<xml_diff>
--- a/openlaw.xlsx
+++ b/openlaw.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/6a089eb5b0364d8d/Project/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="11_DD26AE48F0DFD88A9E9D1E9F38AED5108DD1367D" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="4" documentId="11_DD26AE48F0DFD88A9E9D1E9F38AED5108DD1367D" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{E2C5795E-6708-D04E-9D51-4E5D0C0CDB21}"/>
   <bookViews>
-    <workbookView xWindow="7700" yWindow="3760" windowWidth="51200" windowHeight="26580" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="14400" yWindow="3060" windowWidth="51200" windowHeight="26580" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet0" sheetId="1" r:id="rId1"/>
@@ -2847,8 +2847,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AK51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="P23" sqref="P23"/>
+    <sheetView tabSelected="1" topLeftCell="V1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>